<commit_message>
added the dates to the usg-ground-based-comparison files and created plots for speed/radiant diff against date... promising!
</commit_message>
<xml_diff>
--- a/speed_radiant_difference/usg-ground-based-comparison/usg-ground-based-comparison_EDITED.xlsx
+++ b/speed_radiant_difference/usg-ground-based-comparison/usg-ground-based-comparison_EDITED.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="104">
   <si>
     <t xml:space="preserve">Event</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t xml:space="preserve">Meteorite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
   </si>
   <si>
     <t xml:space="preserve">Length (km)</t>
@@ -566,11 +569,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.00E+00"/>
+    <numFmt numFmtId="168" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="169" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -885,7 +890,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1006,6 +1011,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="12" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
@@ -1016,6 +1025,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1158,10 +1171,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="AF43" activeCellId="0" sqref="AF43"/>
+      <selection pane="bottomLeft" activeCell="AF38" activeCellId="0" sqref="AF38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.57"/>
@@ -1179,7 +1192,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="30" min="30" style="0" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="67.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="67.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1282,11 +1295,14 @@
       <c r="AI1" s="0" t="s">
         <v>31</v>
       </c>
+      <c r="AJ1" s="0" t="s">
+        <v>32</v>
+      </c>
       <c r="AL1" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1298,10 +1314,10 @@
       <c r="I2" s="8"/>
       <c r="J2" s="9"/>
       <c r="K2" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
@@ -1321,38 +1337,38 @@
       <c r="AB2" s="6"/>
       <c r="AC2" s="7"/>
       <c r="AD2" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AE2" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
       <c r="J3" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K3" s="12"/>
       <c r="L3" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M3" s="12" t="n">
         <f aca="false">180/3.14159265</f>
@@ -1363,54 +1379,54 @@
         <v>0.0174532925</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P3" s="15"/>
       <c r="Q3" s="14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R3" s="14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S3" s="14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="T3" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="U3" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="V3" s="15"/>
       <c r="W3" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="X3" s="16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y3" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Z3" s="16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AA3" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AB3" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AC3" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AD3" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AE3" s="16"/>
     </row>
     <row r="4" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B4" s="19" t="n">
         <f aca="false">281.7</f>
@@ -1492,19 +1508,19 @@
       </c>
       <c r="AC4" s="23"/>
       <c r="AD4" s="20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AE4" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="AI4" s="0" t="s">
         <v>49</v>
       </c>
+      <c r="AJ4" s="0" t="s">
+        <v>50</v>
+      </c>
       <c r="AL4" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="18"/>
       <c r="B5" s="24" t="n">
         <f aca="false">281.3</f>
@@ -1591,23 +1607,26 @@
       </c>
       <c r="AD5" s="25"/>
       <c r="AE5" s="25"/>
-      <c r="AF5" s="0" t="n">
-        <f aca="false">(AG5 - AH5)/COS(RADIANS(C4))</f>
+      <c r="AF5" s="30" t="n">
+        <v>39728</v>
+      </c>
+      <c r="AG5" s="0" t="n">
+        <f aca="false">(AH5 - AI5)/COS(RADIANS(C4))</f>
         <v>93.5617408052188</v>
       </c>
-      <c r="AG5" s="0" t="n">
+      <c r="AH5" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="AH5" s="0" t="n">
+      <c r="AI5" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="AI5" s="0" t="s">
-        <v>51</v>
+      <c r="AJ5" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B6" s="19" t="n">
         <v>348.6</v>
@@ -1645,58 +1664,58 @@
       <c r="L6" s="20"/>
       <c r="M6" s="20"/>
       <c r="N6" s="20"/>
-      <c r="O6" s="30" t="n">
+      <c r="O6" s="31" t="n">
         <v>1.23</v>
       </c>
-      <c r="P6" s="30" t="n">
+      <c r="P6" s="31" t="n">
         <v>0.22</v>
       </c>
-      <c r="Q6" s="30" t="n">
+      <c r="Q6" s="31" t="n">
         <v>25.5</v>
       </c>
-      <c r="R6" s="30" t="n">
+      <c r="R6" s="31" t="n">
         <v>238.9</v>
       </c>
-      <c r="S6" s="30" t="n">
+      <c r="S6" s="31" t="n">
         <v>212</v>
       </c>
-      <c r="T6" s="30" t="n">
+      <c r="T6" s="31" t="n">
         <v>0.959</v>
       </c>
-      <c r="U6" s="30" t="n">
+      <c r="U6" s="31" t="n">
         <v>1.5</v>
       </c>
-      <c r="V6" s="30" t="n">
+      <c r="V6" s="31" t="n">
         <v>5.09</v>
       </c>
-      <c r="W6" s="30" t="n">
+      <c r="W6" s="31" t="n">
         <v>0.31</v>
       </c>
-      <c r="X6" s="31" t="n">
+      <c r="X6" s="32" t="n">
         <v>8000</v>
       </c>
-      <c r="Y6" s="30" t="n">
+      <c r="Y6" s="31" t="n">
         <v>1.7</v>
       </c>
-      <c r="Z6" s="30" t="n">
+      <c r="Z6" s="31" t="n">
         <v>18</v>
       </c>
-      <c r="AA6" s="32"/>
-      <c r="AB6" s="30" t="n">
+      <c r="AA6" s="33"/>
+      <c r="AB6" s="31" t="n">
         <v>31</v>
       </c>
-      <c r="AC6" s="32"/>
-      <c r="AD6" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE6" s="30" t="s">
+      <c r="AC6" s="33"/>
+      <c r="AD6" s="31" t="s">
         <v>54</v>
       </c>
+      <c r="AE6" s="31" t="s">
+        <v>55</v>
+      </c>
       <c r="AL6" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="18"/>
       <c r="B7" s="24" t="n">
         <v>330.6</v>
@@ -1782,19 +1801,22 @@
       </c>
       <c r="AD7" s="25"/>
       <c r="AE7" s="25"/>
-      <c r="AF7" s="0" t="n">
+      <c r="AF7" s="34" t="n">
+        <v>39773</v>
+      </c>
+      <c r="AG7" s="0" t="n">
         <v>54.3</v>
       </c>
-      <c r="AG7" s="0" t="n">
+      <c r="AH7" s="0" t="n">
         <v>81</v>
       </c>
-      <c r="AH7" s="0" t="n">
+      <c r="AI7" s="0" t="n">
         <v>12.7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B8" s="19" t="n">
         <v>103.5</v>
@@ -1828,58 +1850,58 @@
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
       <c r="N8" s="20"/>
-      <c r="O8" s="30" t="n">
+      <c r="O8" s="31" t="n">
         <v>1.72</v>
       </c>
-      <c r="P8" s="30" t="n">
+      <c r="P8" s="31" t="n">
         <v>0.571</v>
       </c>
-      <c r="Q8" s="30" t="n">
+      <c r="Q8" s="31" t="n">
         <v>5</v>
       </c>
-      <c r="R8" s="30" t="n">
+      <c r="R8" s="31" t="n">
         <v>326.46</v>
       </c>
-      <c r="S8" s="30" t="n">
+      <c r="S8" s="31" t="n">
         <v>107.7</v>
       </c>
-      <c r="T8" s="30" t="n">
+      <c r="T8" s="31" t="n">
         <v>0.738</v>
       </c>
-      <c r="U8" s="30" t="n">
+      <c r="U8" s="31" t="n">
         <v>2.7</v>
       </c>
-      <c r="V8" s="30" t="n">
+      <c r="V8" s="31" t="n">
         <v>3.97</v>
       </c>
-      <c r="W8" s="30" t="n">
+      <c r="W8" s="31" t="n">
         <v>500</v>
       </c>
-      <c r="X8" s="31" t="n">
+      <c r="X8" s="32" t="n">
         <v>12000000</v>
       </c>
-      <c r="Y8" s="30" t="n">
+      <c r="Y8" s="31" t="n">
         <v>19</v>
       </c>
-      <c r="Z8" s="30" t="n">
+      <c r="Z8" s="31" t="n">
         <v>19</v>
       </c>
-      <c r="AA8" s="32"/>
-      <c r="AB8" s="30" t="n">
+      <c r="AA8" s="33"/>
+      <c r="AB8" s="31" t="n">
         <v>30</v>
       </c>
-      <c r="AC8" s="32"/>
-      <c r="AD8" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE8" s="30" t="s">
+      <c r="AC8" s="33"/>
+      <c r="AD8" s="31" t="s">
         <v>58</v>
       </c>
+      <c r="AE8" s="31" t="s">
+        <v>59</v>
+      </c>
       <c r="AL8" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="18"/>
       <c r="B9" s="24" t="n">
         <v>99.9</v>
@@ -1965,19 +1987,22 @@
       </c>
       <c r="AD9" s="25"/>
       <c r="AE9" s="25"/>
-      <c r="AF9" s="0" t="n">
+      <c r="AF9" s="34" t="n">
+        <v>41320</v>
+      </c>
+      <c r="AG9" s="0" t="n">
         <v>222.7</v>
       </c>
-      <c r="AG9" s="0" t="n">
+      <c r="AH9" s="0" t="n">
         <v>95.1</v>
       </c>
-      <c r="AH9" s="0" t="n">
+      <c r="AI9" s="0" t="n">
         <v>12.6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B10" s="19" t="n">
         <v>297.14</v>
@@ -2015,61 +2040,61 @@
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
       <c r="N10" s="20"/>
-      <c r="O10" s="30" t="n">
+      <c r="O10" s="31" t="n">
         <v>2.71</v>
       </c>
-      <c r="P10" s="30" t="n">
+      <c r="P10" s="31" t="n">
         <v>0.647</v>
       </c>
-      <c r="Q10" s="30" t="n">
+      <c r="Q10" s="31" t="n">
         <v>2</v>
       </c>
-      <c r="R10" s="30" t="n">
+      <c r="R10" s="31" t="n">
         <v>340.07</v>
       </c>
-      <c r="S10" s="30" t="n">
+      <c r="S10" s="31" t="n">
         <v>204.2</v>
       </c>
-      <c r="T10" s="30" t="n">
+      <c r="T10" s="31" t="n">
         <v>0.957</v>
       </c>
-      <c r="U10" s="30" t="n">
+      <c r="U10" s="31" t="n">
         <v>4.46</v>
       </c>
-      <c r="V10" s="30" t="n">
+      <c r="V10" s="31" t="n">
         <v>3.02</v>
       </c>
-      <c r="W10" s="30" t="n">
+      <c r="W10" s="31" t="n">
         <v>0.13</v>
       </c>
-      <c r="X10" s="31" t="n">
+      <c r="X10" s="32" t="n">
         <v>3500</v>
       </c>
-      <c r="Y10" s="30" t="n">
+      <c r="Y10" s="31" t="n">
         <v>1.2</v>
       </c>
-      <c r="Z10" s="30" t="n">
+      <c r="Z10" s="31" t="n">
         <v>15</v>
       </c>
-      <c r="AA10" s="32"/>
-      <c r="AB10" s="30" t="n">
+      <c r="AA10" s="33"/>
+      <c r="AB10" s="31" t="n">
         <v>36</v>
       </c>
-      <c r="AC10" s="32"/>
-      <c r="AD10" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE10" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI10" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="AL10" s="33" t="s">
+      <c r="AC10" s="33"/>
+      <c r="AD10" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE10" s="31" t="s">
         <v>62</v>
       </c>
+      <c r="AJ10" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL10" s="35" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="18"/>
       <c r="B11" s="24" t="n">
         <v>257.6</v>
@@ -2154,23 +2179,26 @@
       </c>
       <c r="AD11" s="25"/>
       <c r="AE11" s="25"/>
-      <c r="AF11" s="0" t="n">
-        <f aca="false">(AG11 - AH11)/COS(RADIANS(C10))</f>
+      <c r="AF11" s="34" t="n">
+        <v>40237</v>
+      </c>
+      <c r="AG11" s="0" t="n">
+        <f aca="false">(AH11 - AI11)/COS(RADIANS(C10))</f>
         <v>91.7374267127706</v>
       </c>
-      <c r="AG11" s="0" t="n">
+      <c r="AH11" s="0" t="n">
         <v>68.3</v>
       </c>
-      <c r="AH11" s="0" t="n">
+      <c r="AI11" s="0" t="n">
         <v>17.4</v>
       </c>
-      <c r="AI11" s="0" t="s">
-        <v>63</v>
+      <c r="AJ11" s="0" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B12" s="19" t="n">
         <v>95.19</v>
@@ -2204,34 +2232,34 @@
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
       <c r="N12" s="20"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="30"/>
-      <c r="S12" s="30"/>
-      <c r="T12" s="30"/>
-      <c r="U12" s="30"/>
-      <c r="V12" s="30"/>
-      <c r="W12" s="30"/>
-      <c r="X12" s="31"/>
-      <c r="Y12" s="30"/>
-      <c r="Z12" s="30" t="n">
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="31"/>
+      <c r="T12" s="31"/>
+      <c r="U12" s="31"/>
+      <c r="V12" s="31"/>
+      <c r="W12" s="31"/>
+      <c r="X12" s="32"/>
+      <c r="Y12" s="31"/>
+      <c r="Z12" s="31" t="n">
         <v>17</v>
       </c>
-      <c r="AA12" s="32"/>
-      <c r="AB12" s="30" t="n">
+      <c r="AA12" s="33"/>
+      <c r="AB12" s="31" t="n">
         <v>27.8</v>
       </c>
-      <c r="AC12" s="32"/>
-      <c r="AD12" s="30"/>
-      <c r="AE12" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="AL12" s="34" t="s">
+      <c r="AC12" s="33"/>
+      <c r="AD12" s="31"/>
+      <c r="AE12" s="31" t="s">
         <v>66</v>
       </c>
+      <c r="AL12" s="36" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="18"/>
       <c r="B13" s="24" t="n">
         <v>95.89</v>
@@ -2295,19 +2323,22 @@
       </c>
       <c r="AD13" s="25"/>
       <c r="AE13" s="25"/>
-      <c r="AF13" s="0" t="n">
+      <c r="AF13" s="34" t="n">
+        <v>43253</v>
+      </c>
+      <c r="AG13" s="0" t="n">
         <v>124.8</v>
       </c>
-      <c r="AG13" s="0" t="n">
+      <c r="AH13" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="AH13" s="0" t="n">
+      <c r="AI13" s="0" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B14" s="19" t="n">
         <v>177.566</v>
@@ -2341,32 +2372,32 @@
       <c r="L14" s="20"/>
       <c r="M14" s="20"/>
       <c r="N14" s="20"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="30"/>
-      <c r="T14" s="30"/>
-      <c r="U14" s="30"/>
-      <c r="V14" s="30"/>
-      <c r="W14" s="30"/>
-      <c r="X14" s="31"/>
-      <c r="Y14" s="30"/>
-      <c r="Z14" s="35" t="n">
+      <c r="O14" s="31"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="31"/>
+      <c r="R14" s="31"/>
+      <c r="S14" s="31"/>
+      <c r="T14" s="31"/>
+      <c r="U14" s="31"/>
+      <c r="V14" s="31"/>
+      <c r="W14" s="31"/>
+      <c r="X14" s="32"/>
+      <c r="Y14" s="31"/>
+      <c r="Z14" s="37" t="n">
         <v>16.5</v>
       </c>
       <c r="AA14" s="29"/>
-      <c r="AB14" s="35" t="n">
+      <c r="AB14" s="37" t="n">
         <v>27</v>
       </c>
-      <c r="AC14" s="32"/>
-      <c r="AD14" s="30"/>
-      <c r="AE14" s="30"/>
+      <c r="AC14" s="33"/>
+      <c r="AD14" s="31"/>
+      <c r="AE14" s="31"/>
       <c r="AL14" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="18"/>
       <c r="B15" s="24" t="n">
         <v>280.1</v>
@@ -2414,14 +2445,14 @@
       <c r="W15" s="25"/>
       <c r="X15" s="28"/>
       <c r="Y15" s="25"/>
-      <c r="Z15" s="36" t="n">
+      <c r="Z15" s="38" t="n">
         <v>14.7</v>
       </c>
       <c r="AA15" s="29" t="n">
         <f aca="false">Z15-Z14</f>
         <v>-1.8</v>
       </c>
-      <c r="AB15" s="36" t="n">
+      <c r="AB15" s="38" t="n">
         <v>36</v>
       </c>
       <c r="AC15" s="29" t="n">
@@ -2430,19 +2461,22 @@
       </c>
       <c r="AD15" s="25"/>
       <c r="AE15" s="25"/>
-      <c r="AF15" s="0" t="n">
+      <c r="AF15" s="34" t="n">
+        <v>42983</v>
+      </c>
+      <c r="AG15" s="0" t="n">
         <v>123</v>
       </c>
-      <c r="AG15" s="0" t="n">
+      <c r="AH15" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="AH15" s="0" t="n">
+      <c r="AI15" s="0" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B16" s="19" t="n">
         <v>6.74</v>
@@ -2476,35 +2510,35 @@
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>
       <c r="N16" s="20"/>
-      <c r="O16" s="30"/>
-      <c r="P16" s="30"/>
-      <c r="Q16" s="30"/>
-      <c r="R16" s="30"/>
-      <c r="S16" s="30"/>
-      <c r="T16" s="30"/>
-      <c r="U16" s="30"/>
-      <c r="V16" s="30"/>
-      <c r="W16" s="30"/>
-      <c r="X16" s="31"/>
-      <c r="Y16" s="30"/>
-      <c r="Z16" s="30" t="n">
+      <c r="O16" s="31"/>
+      <c r="P16" s="31"/>
+      <c r="Q16" s="31"/>
+      <c r="R16" s="31"/>
+      <c r="S16" s="31"/>
+      <c r="T16" s="31"/>
+      <c r="U16" s="31"/>
+      <c r="V16" s="31"/>
+      <c r="W16" s="31"/>
+      <c r="X16" s="32"/>
+      <c r="Y16" s="31"/>
+      <c r="Z16" s="31" t="n">
         <v>9.6</v>
       </c>
-      <c r="AA16" s="32"/>
-      <c r="AB16" s="30" t="n">
+      <c r="AA16" s="33"/>
+      <c r="AB16" s="31" t="n">
         <v>25.7</v>
       </c>
-      <c r="AC16" s="32"/>
-      <c r="AD16" s="30"/>
-      <c r="AE16" s="30"/>
-      <c r="AI16" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="AL16" s="34" t="s">
+      <c r="AC16" s="33"/>
+      <c r="AD16" s="31"/>
+      <c r="AE16" s="31"/>
+      <c r="AJ16" s="0" t="s">
         <v>71</v>
       </c>
+      <c r="AL16" s="36" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="18"/>
       <c r="B17" s="24" t="n">
         <v>11.6</v>
@@ -2568,24 +2602,27 @@
       </c>
       <c r="AD17" s="25"/>
       <c r="AE17" s="25"/>
-      <c r="AF17" s="0" t="n">
+      <c r="AF17" s="34" t="n">
+        <v>42916</v>
+      </c>
+      <c r="AG17" s="0" t="n">
         <f aca="false">(86.782 - 25.648)/COS(RADIANS(C16)) + (5.46 - 4.61) * 0.85</f>
         <v>64.7185062155899</v>
       </c>
-      <c r="AG17" s="0" t="n">
+      <c r="AH17" s="0" t="n">
         <v>86.782</v>
       </c>
-      <c r="AH17" s="0" t="n">
-        <f aca="false">AG17 - AF17 * COS(RADIANS(17.2))</f>
+      <c r="AI17" s="0" t="n">
+        <f aca="false">AH17 - AG17 * COS(RADIANS(17.2))</f>
         <v>24.9578113833666</v>
       </c>
-      <c r="AI17" s="0" t="s">
-        <v>72</v>
+      <c r="AJ17" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B18" s="19" t="n">
         <v>346.41</v>
@@ -2619,35 +2656,35 @@
       <c r="L18" s="20"/>
       <c r="M18" s="20"/>
       <c r="N18" s="20"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="30"/>
-      <c r="R18" s="30"/>
-      <c r="S18" s="30"/>
-      <c r="T18" s="30"/>
-      <c r="U18" s="30"/>
-      <c r="V18" s="30"/>
-      <c r="W18" s="30"/>
-      <c r="X18" s="31"/>
-      <c r="Y18" s="30"/>
-      <c r="Z18" s="30" t="n">
+      <c r="O18" s="31"/>
+      <c r="P18" s="31"/>
+      <c r="Q18" s="31"/>
+      <c r="R18" s="31"/>
+      <c r="S18" s="31"/>
+      <c r="T18" s="31"/>
+      <c r="U18" s="31"/>
+      <c r="V18" s="31"/>
+      <c r="W18" s="31"/>
+      <c r="X18" s="32"/>
+      <c r="Y18" s="31"/>
+      <c r="Z18" s="31" t="n">
         <v>13.4</v>
       </c>
-      <c r="AA18" s="32"/>
-      <c r="AB18" s="30" t="n">
+      <c r="AA18" s="33"/>
+      <c r="AB18" s="31" t="n">
         <v>40.2</v>
       </c>
-      <c r="AC18" s="32"/>
-      <c r="AD18" s="30"/>
-      <c r="AE18" s="30"/>
-      <c r="AI18" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="AL18" s="34" t="s">
-        <v>71</v>
+      <c r="AC18" s="33"/>
+      <c r="AD18" s="31"/>
+      <c r="AE18" s="31"/>
+      <c r="AJ18" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL18" s="36" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="18"/>
       <c r="B19" s="24" t="n">
         <v>331.7</v>
@@ -2711,20 +2748,23 @@
       </c>
       <c r="AD19" s="25"/>
       <c r="AE19" s="25"/>
-      <c r="AF19" s="0" t="n">
-        <f aca="false">(AG19 - AH19)/COS(RADIANS(C18))</f>
+      <c r="AF19" s="34" t="n">
+        <v>42006</v>
+      </c>
+      <c r="AG19" s="0" t="n">
+        <f aca="false">(AH19 - AI19)/COS(RADIANS(C18))</f>
         <v>145.889068154938</v>
       </c>
-      <c r="AG19" s="0" t="n">
+      <c r="AH19" s="0" t="n">
         <v>83.317</v>
       </c>
-      <c r="AH19" s="0" t="n">
+      <c r="AI19" s="0" t="n">
         <v>33.42</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="37" t="s">
-        <v>74</v>
+      <c r="A20" s="39" t="s">
+        <v>75</v>
       </c>
       <c r="B20" s="19" t="n">
         <v>232.2</v>
@@ -2758,36 +2798,36 @@
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
       <c r="N20" s="20"/>
-      <c r="O20" s="30"/>
-      <c r="P20" s="30"/>
-      <c r="Q20" s="30"/>
-      <c r="R20" s="30"/>
-      <c r="S20" s="30"/>
-      <c r="T20" s="30"/>
-      <c r="U20" s="30"/>
-      <c r="V20" s="30"/>
-      <c r="W20" s="30"/>
-      <c r="X20" s="31"/>
-      <c r="Y20" s="30"/>
-      <c r="Z20" s="30" t="n">
+      <c r="O20" s="31"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="31"/>
+      <c r="R20" s="31"/>
+      <c r="S20" s="31"/>
+      <c r="T20" s="31"/>
+      <c r="U20" s="31"/>
+      <c r="V20" s="31"/>
+      <c r="W20" s="31"/>
+      <c r="X20" s="32"/>
+      <c r="Y20" s="31"/>
+      <c r="Z20" s="31" t="n">
         <v>27.76</v>
       </c>
-      <c r="AA20" s="32"/>
-      <c r="AB20" s="30" t="n">
+      <c r="AA20" s="33"/>
+      <c r="AB20" s="31" t="n">
         <v>42.8</v>
       </c>
-      <c r="AC20" s="32"/>
-      <c r="AD20" s="30"/>
-      <c r="AE20" s="30"/>
-      <c r="AI20" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="AL20" s="34" t="s">
-        <v>75</v>
+      <c r="AC20" s="33"/>
+      <c r="AD20" s="31"/>
+      <c r="AE20" s="31"/>
+      <c r="AJ20" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL20" s="36" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="37"/>
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="39"/>
       <c r="B21" s="24" t="n">
         <v>222.9</v>
       </c>
@@ -2849,20 +2889,23 @@
       </c>
       <c r="AD21" s="25"/>
       <c r="AE21" s="25"/>
-      <c r="AF21" s="0" t="n">
-        <f aca="false">(AG21 - AH21)/COS(RADIANS(C20))</f>
+      <c r="AF21" s="34" t="n">
+        <v>42011</v>
+      </c>
+      <c r="AG21" s="0" t="n">
+        <f aca="false">(AH21 - AI21)/COS(RADIANS(C20))</f>
         <v>68.6365286797908</v>
       </c>
-      <c r="AG21" s="0" t="n">
+      <c r="AH21" s="0" t="n">
         <v>85.5</v>
       </c>
-      <c r="AH21" s="0" t="n">
+      <c r="AI21" s="0" t="n">
         <v>38.69</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="37" t="s">
-        <v>76</v>
+      <c r="A22" s="39" t="s">
+        <v>77</v>
       </c>
       <c r="B22" s="19" t="n">
         <v>188.1</v>
@@ -2896,35 +2939,35 @@
       <c r="L22" s="20"/>
       <c r="M22" s="20"/>
       <c r="N22" s="20"/>
-      <c r="O22" s="30"/>
-      <c r="P22" s="30"/>
-      <c r="Q22" s="30"/>
-      <c r="R22" s="30"/>
-      <c r="S22" s="30"/>
-      <c r="T22" s="30"/>
-      <c r="U22" s="30"/>
-      <c r="V22" s="30"/>
-      <c r="W22" s="30"/>
-      <c r="X22" s="31"/>
-      <c r="Y22" s="30"/>
-      <c r="Z22" s="30" t="n">
+      <c r="O22" s="31"/>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="31"/>
+      <c r="R22" s="31"/>
+      <c r="S22" s="31"/>
+      <c r="T22" s="31"/>
+      <c r="U22" s="31"/>
+      <c r="V22" s="31"/>
+      <c r="W22" s="31"/>
+      <c r="X22" s="32"/>
+      <c r="Y22" s="31"/>
+      <c r="Z22" s="31" t="n">
         <v>19.43</v>
       </c>
-      <c r="AA22" s="32"/>
-      <c r="AB22" s="30" t="n">
+      <c r="AA22" s="33"/>
+      <c r="AB22" s="31" t="n">
         <v>40.7</v>
       </c>
-      <c r="AC22" s="32"/>
-      <c r="AD22" s="30"/>
-      <c r="AE22" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="AL22" s="34" t="s">
+      <c r="AC22" s="33"/>
+      <c r="AD22" s="31"/>
+      <c r="AE22" s="31" t="s">
         <v>78</v>
       </c>
+      <c r="AL22" s="36" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="37"/>
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="39"/>
       <c r="B23" s="24" t="n">
         <v>188.5</v>
       </c>
@@ -2987,19 +3030,22 @@
       </c>
       <c r="AD23" s="25"/>
       <c r="AE23" s="25"/>
-      <c r="AF23" s="0" t="n">
+      <c r="AF23" s="34" t="n">
+        <v>43720</v>
+      </c>
+      <c r="AG23" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="AG23" s="0" t="n">
+      <c r="AH23" s="0" t="n">
         <v>71.84</v>
       </c>
-      <c r="AH23" s="0" t="n">
+      <c r="AI23" s="0" t="n">
         <v>35.3</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="37" t="s">
-        <v>79</v>
+      <c r="A24" s="39" t="s">
+        <v>80</v>
       </c>
       <c r="B24" s="19" t="n">
         <v>156.5</v>
@@ -3033,38 +3079,38 @@
       <c r="L24" s="20"/>
       <c r="M24" s="20"/>
       <c r="N24" s="20"/>
-      <c r="O24" s="30"/>
-      <c r="P24" s="30"/>
-      <c r="Q24" s="30"/>
-      <c r="R24" s="30"/>
-      <c r="S24" s="30"/>
-      <c r="T24" s="30"/>
-      <c r="U24" s="30"/>
-      <c r="V24" s="30"/>
-      <c r="W24" s="30"/>
-      <c r="X24" s="31"/>
-      <c r="Y24" s="30"/>
-      <c r="Z24" s="30" t="n">
+      <c r="O24" s="31"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="31"/>
+      <c r="R24" s="31"/>
+      <c r="S24" s="31"/>
+      <c r="T24" s="31"/>
+      <c r="U24" s="31"/>
+      <c r="V24" s="31"/>
+      <c r="W24" s="31"/>
+      <c r="X24" s="32"/>
+      <c r="Y24" s="31"/>
+      <c r="Z24" s="31" t="n">
         <v>22.11</v>
       </c>
-      <c r="AA24" s="32"/>
-      <c r="AB24" s="30" t="n">
+      <c r="AA24" s="33"/>
+      <c r="AB24" s="31" t="n">
         <v>35</v>
       </c>
-      <c r="AC24" s="32"/>
-      <c r="AD24" s="30"/>
-      <c r="AE24" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="AI24" s="0" t="s">
-        <v>49</v>
+      <c r="AC24" s="33"/>
+      <c r="AD24" s="31"/>
+      <c r="AE24" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ24" s="0" t="s">
+        <v>50</v>
       </c>
       <c r="AL24" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="37"/>
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="39"/>
       <c r="B25" s="24" t="n">
         <v>155</v>
       </c>
@@ -3127,20 +3173,23 @@
       </c>
       <c r="AD25" s="25"/>
       <c r="AE25" s="25"/>
-      <c r="AF25" s="0" t="n">
-        <f aca="false">(AG25 - AH25)/COS(RADIANS(C24))</f>
+      <c r="AF25" s="34" t="n">
+        <v>43889</v>
+      </c>
+      <c r="AG25" s="0" t="n">
+        <f aca="false">(AH25 - AI25)/COS(RADIANS(C24))</f>
         <v>69.5989494539676</v>
       </c>
-      <c r="AG25" s="0" t="n">
+      <c r="AH25" s="0" t="n">
         <v>68.7</v>
       </c>
-      <c r="AH25" s="0" t="n">
+      <c r="AI25" s="0" t="n">
         <v>17.1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="37" t="s">
-        <v>82</v>
+      <c r="A26" s="39" t="s">
+        <v>83</v>
       </c>
       <c r="B26" s="19" t="n">
         <v>319.6</v>
@@ -3174,35 +3223,35 @@
       <c r="L26" s="20"/>
       <c r="M26" s="20"/>
       <c r="N26" s="20"/>
-      <c r="O26" s="30"/>
-      <c r="P26" s="30"/>
-      <c r="Q26" s="30"/>
-      <c r="R26" s="30"/>
-      <c r="S26" s="30"/>
-      <c r="T26" s="30"/>
-      <c r="U26" s="30"/>
-      <c r="V26" s="30"/>
-      <c r="W26" s="30"/>
-      <c r="X26" s="31"/>
-      <c r="Y26" s="30"/>
-      <c r="Z26" s="30" t="n">
+      <c r="O26" s="31"/>
+      <c r="P26" s="31"/>
+      <c r="Q26" s="31"/>
+      <c r="R26" s="31"/>
+      <c r="S26" s="31"/>
+      <c r="T26" s="31"/>
+      <c r="U26" s="31"/>
+      <c r="V26" s="31"/>
+      <c r="W26" s="31"/>
+      <c r="X26" s="32"/>
+      <c r="Y26" s="31"/>
+      <c r="Z26" s="31" t="n">
         <v>17.1</v>
       </c>
-      <c r="AA26" s="32"/>
-      <c r="AB26" s="30" t="n">
+      <c r="AA26" s="33"/>
+      <c r="AB26" s="31" t="n">
         <v>36.5</v>
       </c>
-      <c r="AC26" s="32"/>
-      <c r="AD26" s="30"/>
-      <c r="AE26" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="AL26" s="34" t="s">
-        <v>83</v>
+      <c r="AC26" s="33"/>
+      <c r="AD26" s="31"/>
+      <c r="AE26" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL26" s="36" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="37"/>
+      <c r="A27" s="39"/>
       <c r="B27" s="24" t="n">
         <v>48.8</v>
       </c>
@@ -3265,22 +3314,25 @@
       </c>
       <c r="AD27" s="25"/>
       <c r="AE27" s="25"/>
-      <c r="AF27" s="0" t="n">
+      <c r="AF27" s="34" t="n">
+        <v>42249</v>
+      </c>
+      <c r="AG27" s="0" t="n">
         <v>31.6</v>
       </c>
-      <c r="AG27" s="0" t="n">
+      <c r="AH27" s="0" t="n">
         <v>58.4</v>
       </c>
-      <c r="AH27" s="0" t="n">
+      <c r="AI27" s="0" t="n">
         <v>21.3</v>
       </c>
-      <c r="AI27" s="0" t="s">
-        <v>84</v>
+      <c r="AJ27" s="0" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="37" t="s">
-        <v>85</v>
+      <c r="A28" s="39" t="s">
+        <v>86</v>
       </c>
       <c r="B28" s="19" t="n">
         <v>171.8</v>
@@ -3314,38 +3366,38 @@
       <c r="L28" s="20"/>
       <c r="M28" s="20"/>
       <c r="N28" s="20"/>
-      <c r="O28" s="30"/>
-      <c r="P28" s="30"/>
-      <c r="Q28" s="30"/>
-      <c r="R28" s="30"/>
-      <c r="S28" s="30"/>
-      <c r="T28" s="30"/>
-      <c r="U28" s="30"/>
-      <c r="V28" s="30"/>
-      <c r="W28" s="30"/>
-      <c r="X28" s="31"/>
-      <c r="Y28" s="30"/>
-      <c r="Z28" s="30" t="n">
+      <c r="O28" s="31"/>
+      <c r="P28" s="31"/>
+      <c r="Q28" s="31"/>
+      <c r="R28" s="31"/>
+      <c r="S28" s="31"/>
+      <c r="T28" s="31"/>
+      <c r="U28" s="31"/>
+      <c r="V28" s="31"/>
+      <c r="W28" s="31"/>
+      <c r="X28" s="32"/>
+      <c r="Y28" s="31"/>
+      <c r="Z28" s="31" t="n">
         <v>16.6</v>
       </c>
-      <c r="AA28" s="32"/>
-      <c r="AB28" s="30" t="n">
+      <c r="AA28" s="33"/>
+      <c r="AB28" s="31" t="n">
         <v>36.5</v>
       </c>
-      <c r="AC28" s="32"/>
-      <c r="AD28" s="30"/>
-      <c r="AE28" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="AI28" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="AL28" s="34" t="s">
+      <c r="AC28" s="33"/>
+      <c r="AD28" s="31"/>
+      <c r="AE28" s="31" t="s">
         <v>87</v>
       </c>
+      <c r="AJ28" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL28" s="36" t="s">
+        <v>88</v>
+      </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="37"/>
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="39"/>
       <c r="B29" s="24" t="n">
         <v>176.1</v>
       </c>
@@ -3408,20 +3460,23 @@
       </c>
       <c r="AD29" s="25"/>
       <c r="AE29" s="25"/>
-      <c r="AF29" s="0" t="n">
-        <f aca="false">(AG29 - AH29)/COS(RADIANS(C28))</f>
+      <c r="AF29" s="34" t="n">
+        <v>43497</v>
+      </c>
+      <c r="AG29" s="0" t="n">
+        <f aca="false">(AH29 - AI29)/COS(RADIANS(C28))</f>
         <v>63.4077776335121</v>
       </c>
-      <c r="AG29" s="0" t="n">
+      <c r="AH29" s="0" t="n">
         <v>72.24</v>
       </c>
-      <c r="AH29" s="0" t="n">
+      <c r="AI29" s="0" t="n">
         <v>23.313</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="37" t="s">
-        <v>88</v>
+      <c r="A30" s="39" t="s">
+        <v>89</v>
       </c>
       <c r="B30" s="19" t="n">
         <v>243.6</v>
@@ -3455,34 +3510,34 @@
       <c r="L30" s="20"/>
       <c r="M30" s="20"/>
       <c r="N30" s="20"/>
-      <c r="O30" s="30"/>
-      <c r="P30" s="30"/>
-      <c r="Q30" s="30"/>
-      <c r="R30" s="30"/>
-      <c r="S30" s="30"/>
-      <c r="T30" s="30"/>
-      <c r="U30" s="30"/>
-      <c r="V30" s="30"/>
-      <c r="W30" s="30"/>
-      <c r="X30" s="31"/>
-      <c r="Y30" s="30"/>
-      <c r="Z30" s="30" t="n">
+      <c r="O30" s="31"/>
+      <c r="P30" s="31"/>
+      <c r="Q30" s="31"/>
+      <c r="R30" s="31"/>
+      <c r="S30" s="31"/>
+      <c r="T30" s="31"/>
+      <c r="U30" s="31"/>
+      <c r="V30" s="31"/>
+      <c r="W30" s="31"/>
+      <c r="X30" s="32"/>
+      <c r="Y30" s="31"/>
+      <c r="Z30" s="31" t="n">
         <v>17.4</v>
       </c>
-      <c r="AA30" s="32"/>
-      <c r="AB30" s="30"/>
-      <c r="AC30" s="32"/>
-      <c r="AD30" s="30"/>
-      <c r="AE30" s="30"/>
-      <c r="AI30" s="0" t="s">
-        <v>49</v>
+      <c r="AA30" s="33"/>
+      <c r="AB30" s="31"/>
+      <c r="AC30" s="33"/>
+      <c r="AD30" s="31"/>
+      <c r="AE30" s="31"/>
+      <c r="AJ30" s="0" t="s">
+        <v>50</v>
       </c>
       <c r="AL30" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="37"/>
+    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="39"/>
       <c r="B31" s="24" t="n">
         <v>242.2</v>
       </c>
@@ -3540,20 +3595,23 @@
       <c r="AC31" s="29"/>
       <c r="AD31" s="25"/>
       <c r="AE31" s="25"/>
-      <c r="AF31" s="0" t="n">
-        <f aca="false">(AG31 - AH31)/COS(RADIANS(C30))</f>
+      <c r="AF31" s="34" t="n">
+        <v>44142</v>
+      </c>
+      <c r="AG31" s="0" t="n">
+        <f aca="false">(AH31 - AI31)/COS(RADIANS(C30))</f>
         <v>73.4556652656145</v>
       </c>
-      <c r="AG31" s="0" t="n">
+      <c r="AH31" s="0" t="n">
         <v>81.3</v>
       </c>
-      <c r="AH31" s="0" t="n">
+      <c r="AI31" s="0" t="n">
         <v>11.4</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="37" t="s">
-        <v>90</v>
+      <c r="A32" s="39" t="s">
+        <v>91</v>
       </c>
       <c r="B32" s="19" t="n">
         <v>129.3</v>
@@ -3587,31 +3645,31 @@
       <c r="L32" s="20"/>
       <c r="M32" s="20"/>
       <c r="N32" s="20"/>
-      <c r="O32" s="30"/>
-      <c r="P32" s="30"/>
-      <c r="Q32" s="30"/>
-      <c r="R32" s="30"/>
-      <c r="S32" s="30"/>
-      <c r="T32" s="30"/>
-      <c r="U32" s="30"/>
-      <c r="V32" s="30"/>
-      <c r="W32" s="30"/>
-      <c r="X32" s="31"/>
-      <c r="Y32" s="30"/>
-      <c r="Z32" s="30" t="n">
+      <c r="O32" s="31"/>
+      <c r="P32" s="31"/>
+      <c r="Q32" s="31"/>
+      <c r="R32" s="31"/>
+      <c r="S32" s="31"/>
+      <c r="T32" s="31"/>
+      <c r="U32" s="31"/>
+      <c r="V32" s="31"/>
+      <c r="W32" s="31"/>
+      <c r="X32" s="32"/>
+      <c r="Y32" s="31"/>
+      <c r="Z32" s="31" t="n">
         <v>18.6</v>
       </c>
-      <c r="AA32" s="32"/>
-      <c r="AB32" s="30"/>
-      <c r="AC32" s="32"/>
-      <c r="AD32" s="30"/>
-      <c r="AE32" s="30"/>
+      <c r="AA32" s="33"/>
+      <c r="AB32" s="31"/>
+      <c r="AC32" s="33"/>
+      <c r="AD32" s="31"/>
+      <c r="AE32" s="31"/>
       <c r="AL32" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="37"/>
+    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="39"/>
       <c r="B33" s="24" t="n">
         <v>129.8</v>
       </c>
@@ -3670,13 +3728,16 @@
       <c r="AC33" s="29"/>
       <c r="AD33" s="25"/>
       <c r="AE33" s="25"/>
-      <c r="AI33" s="0" t="s">
-        <v>92</v>
+      <c r="AF33" s="34" t="n">
+        <v>44631</v>
+      </c>
+      <c r="AJ33" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="37" t="s">
-        <v>93</v>
+      <c r="A34" s="39" t="s">
+        <v>94</v>
       </c>
       <c r="B34" s="19" t="n">
         <v>109.7</v>
@@ -3710,34 +3771,34 @@
       <c r="L34" s="20"/>
       <c r="M34" s="20"/>
       <c r="N34" s="20"/>
-      <c r="O34" s="30"/>
-      <c r="P34" s="30"/>
-      <c r="Q34" s="30"/>
-      <c r="R34" s="30"/>
-      <c r="S34" s="30"/>
-      <c r="T34" s="30"/>
-      <c r="U34" s="30"/>
-      <c r="V34" s="30"/>
-      <c r="W34" s="30"/>
-      <c r="X34" s="31"/>
-      <c r="Y34" s="30"/>
-      <c r="Z34" s="30" t="n">
+      <c r="O34" s="31"/>
+      <c r="P34" s="31"/>
+      <c r="Q34" s="31"/>
+      <c r="R34" s="31"/>
+      <c r="S34" s="31"/>
+      <c r="T34" s="31"/>
+      <c r="U34" s="31"/>
+      <c r="V34" s="31"/>
+      <c r="W34" s="31"/>
+      <c r="X34" s="32"/>
+      <c r="Y34" s="31"/>
+      <c r="Z34" s="31" t="n">
         <v>16.45</v>
       </c>
-      <c r="AA34" s="32"/>
-      <c r="AB34" s="30"/>
-      <c r="AC34" s="32"/>
-      <c r="AD34" s="30"/>
-      <c r="AE34" s="30"/>
-      <c r="AI34" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="AL34" s="38" t="s">
+      <c r="AA34" s="33"/>
+      <c r="AB34" s="31"/>
+      <c r="AC34" s="33"/>
+      <c r="AD34" s="31"/>
+      <c r="AE34" s="31"/>
+      <c r="AJ34" s="0" t="s">
         <v>95</v>
       </c>
+      <c r="AL34" s="40" t="s">
+        <v>96</v>
+      </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="37"/>
+    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="39"/>
       <c r="B35" s="24" t="n">
         <v>117.9</v>
       </c>
@@ -3788,40 +3849,43 @@
       <c r="AC35" s="29"/>
       <c r="AD35" s="25"/>
       <c r="AE35" s="25"/>
-      <c r="AF35" s="0" t="n">
+      <c r="AF35" s="34" t="n">
+        <v>43638</v>
+      </c>
+      <c r="AG35" s="0" t="n">
         <v>37.835</v>
       </c>
-      <c r="AG35" s="0" t="n">
+      <c r="AH35" s="0" t="n">
         <v>37.62</v>
       </c>
-      <c r="AH35" s="0" t="n">
+      <c r="AI35" s="0" t="n">
         <v>19.92</v>
       </c>
-      <c r="AI35" s="0" t="s">
-        <v>96</v>
+      <c r="AJ35" s="0" t="s">
+        <v>97</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="B36" s="40" t="n">
+    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" s="42" t="n">
         <v>238</v>
       </c>
-      <c r="C36" s="40" t="n">
+      <c r="C36" s="42" t="n">
         <v>12.4</v>
       </c>
-      <c r="D36" s="40"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40" t="n">
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="42" t="n">
         <f aca="false">SIN(C36*$N$3)*COS(B36*$N$3)</f>
         <v>-0.113792387313623</v>
       </c>
-      <c r="G36" s="40" t="n">
+      <c r="G36" s="42" t="n">
         <f aca="false">SIN(B36/$M$3)*SIN(C36/$M$3)</f>
         <v>-0.182105884636612</v>
       </c>
-      <c r="H36" s="40" t="n">
+      <c r="H36" s="42" t="n">
         <f aca="false">COS(C36*$N$3)</f>
         <v>0.976672278387271</v>
       </c>
@@ -3833,50 +3897,50 @@
         <f aca="false">ACOS(I36)*$M$3</f>
         <v>2.40194187465387</v>
       </c>
-      <c r="K36" s="40"/>
-      <c r="L36" s="40"/>
-      <c r="M36" s="40"/>
-      <c r="N36" s="40"/>
-      <c r="O36" s="40"/>
-      <c r="P36" s="40"/>
-      <c r="Q36" s="40"/>
-      <c r="R36" s="40"/>
-      <c r="S36" s="40"/>
-      <c r="T36" s="40"/>
-      <c r="U36" s="40"/>
-      <c r="V36" s="40"/>
-      <c r="W36" s="40"/>
-      <c r="X36" s="41"/>
-      <c r="Y36" s="40"/>
-      <c r="Z36" s="40" t="n">
+      <c r="K36" s="42"/>
+      <c r="L36" s="42"/>
+      <c r="M36" s="42"/>
+      <c r="N36" s="42"/>
+      <c r="O36" s="42"/>
+      <c r="P36" s="42"/>
+      <c r="Q36" s="42"/>
+      <c r="R36" s="42"/>
+      <c r="S36" s="42"/>
+      <c r="T36" s="42"/>
+      <c r="U36" s="42"/>
+      <c r="V36" s="42"/>
+      <c r="W36" s="42"/>
+      <c r="X36" s="43"/>
+      <c r="Y36" s="42"/>
+      <c r="Z36" s="42" t="n">
         <v>14.9</v>
       </c>
-      <c r="AA36" s="42"/>
-      <c r="AB36" s="40" t="n">
+      <c r="AA36" s="44"/>
+      <c r="AB36" s="42" t="n">
         <v>27.2</v>
       </c>
-      <c r="AC36" s="42"/>
-      <c r="AD36" s="40"/>
-      <c r="AE36" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="AI36" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="AL36" s="34" t="s">
+      <c r="AC36" s="44"/>
+      <c r="AD36" s="42"/>
+      <c r="AE36" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ36" s="0" t="s">
         <v>99</v>
       </c>
+      <c r="AL36" s="36" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="39"/>
-      <c r="B37" s="43" t="n">
+    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="41"/>
+      <c r="B37" s="45" t="n">
         <v>237.5</v>
       </c>
-      <c r="C37" s="43" t="n">
+      <c r="C37" s="45" t="n">
         <v>10</v>
       </c>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
       <c r="F37" s="25" t="n">
         <f aca="false">SIN(C37*$N$3)*COS(B37*$N$3)</f>
         <v>-0.0933010984387353</v>
@@ -3889,62 +3953,65 @@
         <f aca="false">COS(C37*$N$3)</f>
         <v>0.984807753046839</v>
       </c>
-      <c r="I37" s="43"/>
-      <c r="J37" s="44"/>
-      <c r="K37" s="43"/>
-      <c r="L37" s="43"/>
-      <c r="M37" s="43"/>
-      <c r="N37" s="43"/>
-      <c r="O37" s="43"/>
-      <c r="P37" s="43"/>
-      <c r="Q37" s="43"/>
-      <c r="R37" s="43"/>
-      <c r="S37" s="43"/>
-      <c r="T37" s="43"/>
-      <c r="U37" s="43"/>
-      <c r="V37" s="43"/>
-      <c r="W37" s="43"/>
-      <c r="X37" s="45"/>
-      <c r="Y37" s="43"/>
-      <c r="Z37" s="43" t="n">
+      <c r="I37" s="45"/>
+      <c r="J37" s="46"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="45"/>
+      <c r="M37" s="45"/>
+      <c r="N37" s="45"/>
+      <c r="O37" s="45"/>
+      <c r="P37" s="45"/>
+      <c r="Q37" s="45"/>
+      <c r="R37" s="45"/>
+      <c r="S37" s="45"/>
+      <c r="T37" s="45"/>
+      <c r="U37" s="45"/>
+      <c r="V37" s="45"/>
+      <c r="W37" s="45"/>
+      <c r="X37" s="47"/>
+      <c r="Y37" s="45"/>
+      <c r="Z37" s="45" t="n">
         <v>14.4</v>
       </c>
       <c r="AA37" s="29" t="n">
         <f aca="false">Z37-Z36</f>
         <v>-0.5</v>
       </c>
-      <c r="AB37" s="43" t="n">
+      <c r="AB37" s="45" t="n">
         <v>27.2</v>
       </c>
       <c r="AC37" s="29" t="n">
         <f aca="false">AB37-AB36</f>
         <v>0</v>
       </c>
-      <c r="AD37" s="43"/>
-      <c r="AE37" s="43"/>
-      <c r="AF37" s="0" t="n">
+      <c r="AD37" s="45"/>
+      <c r="AE37" s="45"/>
+      <c r="AF37" s="34" t="n">
+        <v>43272</v>
+      </c>
+      <c r="AG37" s="0" t="n">
         <v>65.56</v>
       </c>
-      <c r="AG37" s="0" t="n">
+      <c r="AH37" s="0" t="n">
         <v>78.133</v>
       </c>
-      <c r="AH37" s="0" t="n">
+      <c r="AI37" s="0" t="n">
         <v>14.103</v>
       </c>
-      <c r="AI37" s="0" t="s">
-        <v>100</v>
+      <c r="AJ37" s="0" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="36"/>
+      <c r="C39" s="38"/>
       <c r="D39" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="46"/>
+      <c r="C40" s="48"/>
       <c r="D40" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added QLD event to the usg ground baed comparison csv
</commit_message>
<xml_diff>
--- a/speed_radiant_difference/usg-ground-based-comparison/usg-ground-based-comparison_EDITED.xlsx
+++ b/speed_radiant_difference/usg-ground-based-comparison/usg-ground-based-comparison_EDITED.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="107">
   <si>
     <t xml:space="preserve">Event</t>
   </si>
@@ -559,6 +559,15 @@
     <t xml:space="preserve">use speed and LC duration to determine length, use peak brightness height, zenith angle and length to determine begin/end heights; all parameters from paper</t>
   </si>
   <si>
+    <t xml:space="preserve">Queensland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sat-ecf and meteoraudit.txt files are USG data, the report.txt file is ground-based</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Begin/end heights taken from ground-based rather than USG</t>
+  </si>
+  <si>
     <t xml:space="preserve">USG values</t>
   </si>
   <si>
@@ -569,13 +578,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.00E+00"/>
     <numFmt numFmtId="168" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="169" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -890,7 +898,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1025,10 +1033,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1166,15 +1170,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AL40"/>
+  <dimension ref="A1:AL53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="AF38" activeCellId="0" sqref="AF38"/>
+      <selection pane="bottomLeft" activeCell="AG45" activeCellId="0" sqref="AG45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.57"/>
@@ -1192,7 +1196,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="30" min="30" style="0" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="67.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="16.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1801,7 +1805,7 @@
       </c>
       <c r="AD7" s="25"/>
       <c r="AE7" s="25"/>
-      <c r="AF7" s="34" t="n">
+      <c r="AF7" s="30" t="n">
         <v>39773</v>
       </c>
       <c r="AG7" s="0" t="n">
@@ -1987,7 +1991,7 @@
       </c>
       <c r="AD9" s="25"/>
       <c r="AE9" s="25"/>
-      <c r="AF9" s="34" t="n">
+      <c r="AF9" s="30" t="n">
         <v>41320</v>
       </c>
       <c r="AG9" s="0" t="n">
@@ -2090,7 +2094,7 @@
       <c r="AJ10" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="AL10" s="35" t="s">
+      <c r="AL10" s="34" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2179,7 +2183,7 @@
       </c>
       <c r="AD11" s="25"/>
       <c r="AE11" s="25"/>
-      <c r="AF11" s="34" t="n">
+      <c r="AF11" s="30" t="n">
         <v>40237</v>
       </c>
       <c r="AG11" s="0" t="n">
@@ -2255,7 +2259,7 @@
       <c r="AE12" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="AL12" s="36" t="s">
+      <c r="AL12" s="35" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2323,7 +2327,7 @@
       </c>
       <c r="AD13" s="25"/>
       <c r="AE13" s="25"/>
-      <c r="AF13" s="34" t="n">
+      <c r="AF13" s="30" t="n">
         <v>43253</v>
       </c>
       <c r="AG13" s="0" t="n">
@@ -2383,11 +2387,11 @@
       <c r="W14" s="31"/>
       <c r="X14" s="32"/>
       <c r="Y14" s="31"/>
-      <c r="Z14" s="37" t="n">
+      <c r="Z14" s="36" t="n">
         <v>16.5</v>
       </c>
       <c r="AA14" s="29"/>
-      <c r="AB14" s="37" t="n">
+      <c r="AB14" s="36" t="n">
         <v>27</v>
       </c>
       <c r="AC14" s="33"/>
@@ -2445,14 +2449,14 @@
       <c r="W15" s="25"/>
       <c r="X15" s="28"/>
       <c r="Y15" s="25"/>
-      <c r="Z15" s="38" t="n">
+      <c r="Z15" s="37" t="n">
         <v>14.7</v>
       </c>
       <c r="AA15" s="29" t="n">
         <f aca="false">Z15-Z14</f>
         <v>-1.8</v>
       </c>
-      <c r="AB15" s="38" t="n">
+      <c r="AB15" s="37" t="n">
         <v>36</v>
       </c>
       <c r="AC15" s="29" t="n">
@@ -2461,7 +2465,7 @@
       </c>
       <c r="AD15" s="25"/>
       <c r="AE15" s="25"/>
-      <c r="AF15" s="34" t="n">
+      <c r="AF15" s="30" t="n">
         <v>42983</v>
       </c>
       <c r="AG15" s="0" t="n">
@@ -2534,7 +2538,7 @@
       <c r="AJ16" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="AL16" s="36" t="s">
+      <c r="AL16" s="35" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2602,7 +2606,7 @@
       </c>
       <c r="AD17" s="25"/>
       <c r="AE17" s="25"/>
-      <c r="AF17" s="34" t="n">
+      <c r="AF17" s="30" t="n">
         <v>42916</v>
       </c>
       <c r="AG17" s="0" t="n">
@@ -2680,7 +2684,7 @@
       <c r="AJ18" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="AL18" s="36" t="s">
+      <c r="AL18" s="35" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2748,7 +2752,7 @@
       </c>
       <c r="AD19" s="25"/>
       <c r="AE19" s="25"/>
-      <c r="AF19" s="34" t="n">
+      <c r="AF19" s="30" t="n">
         <v>42006</v>
       </c>
       <c r="AG19" s="0" t="n">
@@ -2763,7 +2767,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="38" t="s">
         <v>75</v>
       </c>
       <c r="B20" s="19" t="n">
@@ -2822,12 +2826,12 @@
       <c r="AJ20" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="AL20" s="36" t="s">
+      <c r="AL20" s="35" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="39"/>
+      <c r="A21" s="38"/>
       <c r="B21" s="24" t="n">
         <v>222.9</v>
       </c>
@@ -2889,7 +2893,7 @@
       </c>
       <c r="AD21" s="25"/>
       <c r="AE21" s="25"/>
-      <c r="AF21" s="34" t="n">
+      <c r="AF21" s="30" t="n">
         <v>42011</v>
       </c>
       <c r="AG21" s="0" t="n">
@@ -2904,7 +2908,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="38" t="s">
         <v>77</v>
       </c>
       <c r="B22" s="19" t="n">
@@ -2962,12 +2966,12 @@
       <c r="AE22" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="AL22" s="36" t="s">
+      <c r="AL22" s="35" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="39"/>
+      <c r="A23" s="38"/>
       <c r="B23" s="24" t="n">
         <v>188.5</v>
       </c>
@@ -3030,7 +3034,7 @@
       </c>
       <c r="AD23" s="25"/>
       <c r="AE23" s="25"/>
-      <c r="AF23" s="34" t="n">
+      <c r="AF23" s="30" t="n">
         <v>43720</v>
       </c>
       <c r="AG23" s="0" t="n">
@@ -3044,7 +3048,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="38" t="s">
         <v>80</v>
       </c>
       <c r="B24" s="19" t="n">
@@ -3110,7 +3114,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="39"/>
+      <c r="A25" s="38"/>
       <c r="B25" s="24" t="n">
         <v>155</v>
       </c>
@@ -3173,7 +3177,7 @@
       </c>
       <c r="AD25" s="25"/>
       <c r="AE25" s="25"/>
-      <c r="AF25" s="34" t="n">
+      <c r="AF25" s="30" t="n">
         <v>43889</v>
       </c>
       <c r="AG25" s="0" t="n">
@@ -3188,7 +3192,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="38" t="s">
         <v>83</v>
       </c>
       <c r="B26" s="19" t="n">
@@ -3246,12 +3250,12 @@
       <c r="AE26" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="AL26" s="36" t="s">
+      <c r="AL26" s="35" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="39"/>
+      <c r="A27" s="38"/>
       <c r="B27" s="24" t="n">
         <v>48.8</v>
       </c>
@@ -3314,7 +3318,7 @@
       </c>
       <c r="AD27" s="25"/>
       <c r="AE27" s="25"/>
-      <c r="AF27" s="34" t="n">
+      <c r="AF27" s="30" t="n">
         <v>42249</v>
       </c>
       <c r="AG27" s="0" t="n">
@@ -3331,7 +3335,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="38" t="s">
         <v>86</v>
       </c>
       <c r="B28" s="19" t="n">
@@ -3392,12 +3396,12 @@
       <c r="AJ28" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="AL28" s="36" t="s">
+      <c r="AL28" s="35" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="39"/>
+      <c r="A29" s="38"/>
       <c r="B29" s="24" t="n">
         <v>176.1</v>
       </c>
@@ -3460,7 +3464,7 @@
       </c>
       <c r="AD29" s="25"/>
       <c r="AE29" s="25"/>
-      <c r="AF29" s="34" t="n">
+      <c r="AF29" s="30" t="n">
         <v>43497</v>
       </c>
       <c r="AG29" s="0" t="n">
@@ -3475,7 +3479,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="38" t="s">
         <v>89</v>
       </c>
       <c r="B30" s="19" t="n">
@@ -3537,7 +3541,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="39"/>
+      <c r="A31" s="38"/>
       <c r="B31" s="24" t="n">
         <v>242.2</v>
       </c>
@@ -3591,11 +3595,13 @@
         <f aca="false">Z31-Z30</f>
         <v>-0.699999999999999</v>
       </c>
-      <c r="AB31" s="25"/>
+      <c r="AB31" s="25" t="n">
+        <v>22.3</v>
+      </c>
       <c r="AC31" s="29"/>
       <c r="AD31" s="25"/>
       <c r="AE31" s="25"/>
-      <c r="AF31" s="34" t="n">
+      <c r="AF31" s="30" t="n">
         <v>44142</v>
       </c>
       <c r="AG31" s="0" t="n">
@@ -3610,7 +3616,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="38" t="s">
         <v>91</v>
       </c>
       <c r="B32" s="19" t="n">
@@ -3669,7 +3675,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="39"/>
+      <c r="A33" s="38"/>
       <c r="B33" s="24" t="n">
         <v>129.8</v>
       </c>
@@ -3728,7 +3734,7 @@
       <c r="AC33" s="29"/>
       <c r="AD33" s="25"/>
       <c r="AE33" s="25"/>
-      <c r="AF33" s="34" t="n">
+      <c r="AF33" s="30" t="n">
         <v>44631</v>
       </c>
       <c r="AJ33" s="0" t="s">
@@ -3736,7 +3742,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="39" t="s">
+      <c r="A34" s="38" t="s">
         <v>94</v>
       </c>
       <c r="B34" s="19" t="n">
@@ -3793,12 +3799,12 @@
       <c r="AJ34" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="AL34" s="40" t="s">
+      <c r="AL34" s="39" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="39"/>
+      <c r="A35" s="38"/>
       <c r="B35" s="24" t="n">
         <v>117.9</v>
       </c>
@@ -3849,7 +3855,7 @@
       <c r="AC35" s="29"/>
       <c r="AD35" s="25"/>
       <c r="AE35" s="25"/>
-      <c r="AF35" s="34" t="n">
+      <c r="AF35" s="30" t="n">
         <v>43638</v>
       </c>
       <c r="AG35" s="0" t="n">
@@ -3866,26 +3872,26 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="41" t="s">
+      <c r="A36" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="B36" s="42" t="n">
+      <c r="B36" s="41" t="n">
         <v>238</v>
       </c>
-      <c r="C36" s="42" t="n">
+      <c r="C36" s="41" t="n">
         <v>12.4</v>
       </c>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42" t="n">
+      <c r="D36" s="41"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41" t="n">
         <f aca="false">SIN(C36*$N$3)*COS(B36*$N$3)</f>
         <v>-0.113792387313623</v>
       </c>
-      <c r="G36" s="42" t="n">
+      <c r="G36" s="41" t="n">
         <f aca="false">SIN(B36/$M$3)*SIN(C36/$M$3)</f>
         <v>-0.182105884636612</v>
       </c>
-      <c r="H36" s="42" t="n">
+      <c r="H36" s="41" t="n">
         <f aca="false">COS(C36*$N$3)</f>
         <v>0.976672278387271</v>
       </c>
@@ -3897,50 +3903,50 @@
         <f aca="false">ACOS(I36)*$M$3</f>
         <v>2.40194187465387</v>
       </c>
-      <c r="K36" s="42"/>
-      <c r="L36" s="42"/>
-      <c r="M36" s="42"/>
-      <c r="N36" s="42"/>
-      <c r="O36" s="42"/>
-      <c r="P36" s="42"/>
-      <c r="Q36" s="42"/>
-      <c r="R36" s="42"/>
-      <c r="S36" s="42"/>
-      <c r="T36" s="42"/>
-      <c r="U36" s="42"/>
-      <c r="V36" s="42"/>
-      <c r="W36" s="42"/>
-      <c r="X36" s="43"/>
-      <c r="Y36" s="42"/>
-      <c r="Z36" s="42" t="n">
+      <c r="K36" s="41"/>
+      <c r="L36" s="41"/>
+      <c r="M36" s="41"/>
+      <c r="N36" s="41"/>
+      <c r="O36" s="41"/>
+      <c r="P36" s="41"/>
+      <c r="Q36" s="41"/>
+      <c r="R36" s="41"/>
+      <c r="S36" s="41"/>
+      <c r="T36" s="41"/>
+      <c r="U36" s="41"/>
+      <c r="V36" s="41"/>
+      <c r="W36" s="41"/>
+      <c r="X36" s="42"/>
+      <c r="Y36" s="41"/>
+      <c r="Z36" s="41" t="n">
         <v>14.9</v>
       </c>
-      <c r="AA36" s="44"/>
-      <c r="AB36" s="42" t="n">
+      <c r="AA36" s="43"/>
+      <c r="AB36" s="41" t="n">
         <v>27.2</v>
       </c>
-      <c r="AC36" s="44"/>
-      <c r="AD36" s="42"/>
-      <c r="AE36" s="42" t="s">
+      <c r="AC36" s="43"/>
+      <c r="AD36" s="41"/>
+      <c r="AE36" s="41" t="s">
         <v>87</v>
       </c>
       <c r="AJ36" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="AL36" s="36" t="s">
+      <c r="AL36" s="35" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="41"/>
-      <c r="B37" s="45" t="n">
+      <c r="A37" s="40"/>
+      <c r="B37" s="44" t="n">
         <v>237.5</v>
       </c>
-      <c r="C37" s="45" t="n">
+      <c r="C37" s="44" t="n">
         <v>10</v>
       </c>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
       <c r="F37" s="25" t="n">
         <f aca="false">SIN(C37*$N$3)*COS(B37*$N$3)</f>
         <v>-0.0933010984387353</v>
@@ -3953,40 +3959,40 @@
         <f aca="false">COS(C37*$N$3)</f>
         <v>0.984807753046839</v>
       </c>
-      <c r="I37" s="45"/>
-      <c r="J37" s="46"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="45"/>
-      <c r="M37" s="45"/>
-      <c r="N37" s="45"/>
-      <c r="O37" s="45"/>
-      <c r="P37" s="45"/>
-      <c r="Q37" s="45"/>
-      <c r="R37" s="45"/>
-      <c r="S37" s="45"/>
-      <c r="T37" s="45"/>
-      <c r="U37" s="45"/>
-      <c r="V37" s="45"/>
-      <c r="W37" s="45"/>
-      <c r="X37" s="47"/>
-      <c r="Y37" s="45"/>
-      <c r="Z37" s="45" t="n">
+      <c r="I37" s="44"/>
+      <c r="J37" s="45"/>
+      <c r="K37" s="44"/>
+      <c r="L37" s="44"/>
+      <c r="M37" s="44"/>
+      <c r="N37" s="44"/>
+      <c r="O37" s="44"/>
+      <c r="P37" s="44"/>
+      <c r="Q37" s="44"/>
+      <c r="R37" s="44"/>
+      <c r="S37" s="44"/>
+      <c r="T37" s="44"/>
+      <c r="U37" s="44"/>
+      <c r="V37" s="44"/>
+      <c r="W37" s="44"/>
+      <c r="X37" s="46"/>
+      <c r="Y37" s="44"/>
+      <c r="Z37" s="44" t="n">
         <v>14.4</v>
       </c>
       <c r="AA37" s="29" t="n">
         <f aca="false">Z37-Z36</f>
         <v>-0.5</v>
       </c>
-      <c r="AB37" s="45" t="n">
+      <c r="AB37" s="44" t="n">
         <v>27.2</v>
       </c>
       <c r="AC37" s="29" t="n">
         <f aca="false">AB37-AB36</f>
         <v>0</v>
       </c>
-      <c r="AD37" s="45"/>
-      <c r="AE37" s="45"/>
-      <c r="AF37" s="34" t="n">
+      <c r="AD37" s="44"/>
+      <c r="AE37" s="44"/>
+      <c r="AF37" s="30" t="n">
         <v>43272</v>
       </c>
       <c r="AG37" s="0" t="n">
@@ -4002,18 +4008,155 @@
         <v>101</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="38"/>
-      <c r="D39" s="0" t="s">
+    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="40" t="s">
         <v>102</v>
       </c>
+      <c r="B38" s="41" t="n">
+        <v>99.445</v>
+      </c>
+      <c r="C38" s="41" t="n">
+        <f aca="false">90-41.473</f>
+        <v>48.527</v>
+      </c>
+      <c r="D38" s="41"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="41" t="n">
+        <f aca="false">SIN(C38*$N$3)*COS(B38*$N$3)</f>
+        <v>-0.122955431426187</v>
+      </c>
+      <c r="G38" s="41" t="n">
+        <f aca="false">SIN(B38/$M$3)*SIN(C38/$M$3)</f>
+        <v>0.739110500431005</v>
+      </c>
+      <c r="H38" s="41" t="n">
+        <f aca="false">COS(C38*$N$3)</f>
+        <v>0.662267038312665</v>
+      </c>
+      <c r="I38" s="0" t="n">
+        <f aca="false">F38*F39+G38*G39+H38*H39</f>
+        <v>0.999331193734186</v>
+      </c>
+      <c r="J38" s="21" t="n">
+        <f aca="false">ACOS(I38)*$M$3</f>
+        <v>2.09561744563643</v>
+      </c>
+      <c r="K38" s="41"/>
+      <c r="L38" s="41"/>
+      <c r="M38" s="41"/>
+      <c r="N38" s="41"/>
+      <c r="O38" s="41"/>
+      <c r="P38" s="41"/>
+      <c r="Q38" s="41"/>
+      <c r="R38" s="41"/>
+      <c r="S38" s="41"/>
+      <c r="T38" s="41"/>
+      <c r="U38" s="41"/>
+      <c r="V38" s="41"/>
+      <c r="W38" s="41"/>
+      <c r="X38" s="42"/>
+      <c r="Y38" s="41"/>
+      <c r="Z38" s="41" t="n">
+        <f aca="false">28.6136</f>
+        <v>28.6136</v>
+      </c>
+      <c r="AA38" s="43"/>
+      <c r="AB38" s="41"/>
+      <c r="AC38" s="43"/>
+      <c r="AD38" s="41"/>
+      <c r="AE38" s="41"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="48"/>
-      <c r="D40" s="0" t="s">
+    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="40"/>
+      <c r="B39" s="44" t="n">
+        <v>100.854</v>
+      </c>
+      <c r="C39" s="44" t="n">
+        <v>50.3288</v>
+      </c>
+      <c r="D39" s="44"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="25" t="n">
+        <f aca="false">SIN(C39*$N$3)*COS(B39*$N$3)</f>
+        <v>-0.144943775286197</v>
+      </c>
+      <c r="G39" s="25" t="n">
+        <f aca="false">SIN(B39/$M$3)*SIN(C39/$M$3)</f>
+        <v>0.755950399801812</v>
+      </c>
+      <c r="H39" s="25" t="n">
+        <f aca="false">COS(C39*$N$3)</f>
+        <v>0.638380995209965</v>
+      </c>
+      <c r="I39" s="44"/>
+      <c r="J39" s="45"/>
+      <c r="K39" s="44"/>
+      <c r="L39" s="44"/>
+      <c r="M39" s="44"/>
+      <c r="N39" s="44"/>
+      <c r="O39" s="44"/>
+      <c r="P39" s="44"/>
+      <c r="Q39" s="44"/>
+      <c r="R39" s="44"/>
+      <c r="S39" s="44"/>
+      <c r="T39" s="44"/>
+      <c r="U39" s="44"/>
+      <c r="V39" s="44"/>
+      <c r="W39" s="44"/>
+      <c r="X39" s="46"/>
+      <c r="Y39" s="44"/>
+      <c r="Z39" s="44" t="n">
+        <v>27.9152</v>
+      </c>
+      <c r="AA39" s="29" t="n">
+        <f aca="false">Z39-Z38</f>
+        <v>-0.698400000000003</v>
+      </c>
+      <c r="AB39" s="44" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC39" s="29" t="n">
+        <f aca="false">AB39-AB38</f>
+        <v>29</v>
+      </c>
+      <c r="AD39" s="44"/>
+      <c r="AE39" s="44"/>
+      <c r="AF39" s="30" t="n">
+        <v>45066</v>
+      </c>
+      <c r="AG39" s="0" t="n">
+        <f aca="false">(AH39 - AI39)/COS(RADIANS(C38))</f>
+        <v>67.6561227676651</v>
+      </c>
+      <c r="AH39" s="0" t="n">
+        <v>120.63742</v>
+      </c>
+      <c r="AI39" s="0" t="n">
+        <v>75.831</v>
+      </c>
+      <c r="AJ39" s="0" t="s">
         <v>103</v>
       </c>
     </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AJ40" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="37"/>
+      <c r="D41" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="47"/>
+      <c r="D42" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="32">
     <mergeCell ref="A1:A2"/>

</xml_diff>